<commit_message>
odified mydata excel sheet
</commit_message>
<xml_diff>
--- a/mydata.xlsx
+++ b/mydata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikitharao/Desktop/Lead-Poisoning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikitharao/Desktop/lead-story/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70EE528-4A61-604D-BF48-7CD09323D8BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C878C-5F0B-D44B-A11A-9D9FD17B4102}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,19 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="113">
   <si>
     <t>state</t>
   </si>
@@ -350,13 +358,22 @@
   </si>
   <si>
     <t>All children under 6 years of age living in high-risk areas must be tested for lead poisoning</t>
+  </si>
+  <si>
+    <t>percentage tested</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The President's task Force on Environmental Health Risks and Safety Risks to Children recently released an action plan to help various federal agencies in their efforts to protect children from lead exposure </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -374,6 +391,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,10 +423,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -405,9 +436,19 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -709,34 +750,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="130.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="156.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -746,11 +792,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7">
+        <v>8.2588093684040992E-2</v>
+      </c>
+      <c r="E2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -761,10 +810,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -774,11 +826,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7">
+        <v>0.11418057328712991</v>
+      </c>
+      <c r="E4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -789,10 +844,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -802,11 +860,14 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -816,11 +877,14 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7">
+        <v>6.5874655647382915E-2</v>
+      </c>
+      <c r="E7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -830,11 +894,14 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7">
+        <v>0.31620792988169266</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -844,11 +911,14 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7">
+        <v>0.11695355926125157</v>
+      </c>
+      <c r="E9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -858,11 +928,14 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7">
+        <v>0.250990916597853</v>
+      </c>
+      <c r="E10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -873,10 +946,13 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -886,11 +962,14 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7">
+        <v>0.14923285575791756</v>
+      </c>
+      <c r="E12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -901,10 +980,13 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -915,10 +997,13 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -928,11 +1013,14 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7">
+        <v>0.14134086392636752</v>
+      </c>
+      <c r="E15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -942,11 +1030,14 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7">
+        <v>8.0534775129024336E-2</v>
+      </c>
+      <c r="E16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -957,10 +1048,13 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -971,10 +1065,13 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -984,11 +1081,14 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7">
+        <v>3.2318144299350253E-2</v>
+      </c>
+      <c r="E19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -998,11 +1098,14 @@
       <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7">
+        <v>4.5853078656762178E-2</v>
+      </c>
+      <c r="E20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1013,10 +1116,13 @@
         <v>7</v>
       </c>
       <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1026,11 +1132,14 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7">
+        <v>0.26820227334883856</v>
+      </c>
+      <c r="E22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1040,11 +1149,14 @@
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7">
+        <v>0.47798548483479991</v>
+      </c>
+      <c r="E23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1054,11 +1166,14 @@
       <c r="C24" t="s">
         <v>33</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7">
+        <v>0.20879651797307383</v>
+      </c>
+      <c r="E24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1068,11 +1183,14 @@
       <c r="C25" t="s">
         <v>5</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7">
+        <v>0.21367188705172049</v>
+      </c>
+      <c r="E25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1082,11 +1200,14 @@
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7">
+        <v>0.15447279565756294</v>
+      </c>
+      <c r="E26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1096,11 +1217,14 @@
       <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="7">
+        <v>0.20704783438828134</v>
+      </c>
+      <c r="E27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1111,10 +1235,13 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1125,10 +1252,13 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1139,10 +1269,13 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1152,11 +1285,14 @@
       <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7">
+        <v>0.20111204760167561</v>
+      </c>
+      <c r="E31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1166,11 +1302,14 @@
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7">
+        <v>0.27477866821998204</v>
+      </c>
+      <c r="E32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1180,11 +1319,14 @@
       <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="7">
+        <v>6.5393785926843237E-2</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -1194,11 +1336,14 @@
       <c r="C34" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="7">
+        <v>0.15397906704927361</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -1208,11 +1353,14 @@
       <c r="C35" s="3">
         <v>0.02</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="7">
+        <v>0.45980315877177935</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1222,11 +1370,14 @@
       <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="7">
+        <v>0.11584343547061353</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1237,10 +1388,13 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1250,11 +1404,14 @@
       <c r="C38" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="7">
+        <v>0.19110082396255731</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1264,11 +1421,14 @@
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="7">
+        <v>0.13617274291973086</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1278,11 +1438,14 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="7">
+        <v>6.5096330733140334E-2</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1292,11 +1455,14 @@
       <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -1306,11 +1472,14 @@
       <c r="C42" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="7">
+        <v>0.38637292136361573</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -1320,11 +1489,14 @@
       <c r="C43" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1335,10 +1507,13 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1348,11 +1523,14 @@
       <c r="C45" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="7">
+        <v>0.18386968515210883</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1362,11 +1540,14 @@
       <c r="C46" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -1376,11 +1557,14 @@
       <c r="C47" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1390,11 +1574,14 @@
       <c r="C48" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="7">
+        <v>0.26519978401727862</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1404,11 +1591,14 @@
       <c r="C49" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1418,11 +1608,14 @@
       <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="7">
+        <v>6.0783462755623768E-2</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1432,11 +1625,14 @@
       <c r="C51" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="7">
+        <v>0.1368421052631579</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1446,11 +1642,14 @@
       <c r="C52" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="7">
+        <v>0.21244653881137152</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1460,8 +1659,37 @@
       <c r="C53" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="9">
+        <v>24193364</v>
+      </c>
+      <c r="C54" s="10">
+        <v>3.9999999105930301E-2</v>
+      </c>
+      <c r="D54" s="7">
+        <f>(B56/B54)</f>
+        <v>0.10404233160795663</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="9">
+        <v>2517134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>